<commit_message>
refactor BigInt class: improve addition and subtraction operations, add toInt helper function
</commit_message>
<xml_diff>
--- a/spring-2025/cecs-323/clos.xlsx
+++ b/spring-2025/cecs-323/clos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ca/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ca/development/college/spring-2025/cecs-323/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8D6157-9158-294E-B83C-9B49FC2587E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C55512C-8826-6C4C-B68B-C20CB5A828C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,8 +641,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="E2" s="7">
         <f>(B$1=D2)+(B$6=D2)+(B$10=D2)+(B$14=D2)+(B$18=D2)+(B$22=D2)+(B$26=D2)+(B$31=D2)+(B$36=D2)+(B$41=D2)+(B$45=D2)+(B$49=D2)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>67</v>
@@ -748,7 +748,7 @@
       </c>
       <c r="E5" s="7">
         <f>(B$1=D5)+(B$6=D5)+(B$10=D5)+(B$14=D5)+(B$18=D5)+(B$22=D5)+(B$26=D5)+(B$31=D5)+(B$36=D5)+(B$41=D5)+(B$45=D5)+(B$49=D5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13">
@@ -757,7 +757,7 @@
       </c>
       <c r="B6" s="2">
         <f>ROUND(AVERAGE(B7:B9),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>13</v>
@@ -767,7 +767,7 @@
       </c>
       <c r="E6" s="7">
         <f>(B$1=D6)+(B$6=D6)+(B$10=D6)+(B$14=D6)+(B$18=D6)+(B$22=D6)+(B$26=D6)+(B$31=D6)+(B$36=D6)+(B$41=D6)+(B$45=D6)+(B$49=D6)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13">
@@ -775,7 +775,7 @@
         <v>2.1</v>
       </c>
       <c r="B7" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>47</v>
@@ -821,7 +821,7 @@
       </c>
       <c r="B10" s="2">
         <f>ROUND(AVERAGE(B11:B13),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>15</v>
@@ -829,7 +829,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="13" t="str">
         <f>IF(AND(B1&gt;=3, B6&gt;=3, B10&gt;=3, B14&gt;=3, B22&gt;=3, B26&gt;=3, B50&gt;=3, E3+E2&gt;=9, E9&lt;&gt;"B", E8&lt;&gt;"A"), "C", "")</f>
-        <v/>
+        <v>C</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13">
@@ -853,7 +853,7 @@
         <v>3.2</v>
       </c>
       <c r="B12" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>52</v>
@@ -861,7 +861,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="15" t="str">
         <f>IF(E$2+E$3&lt;6, "F", "")</f>
-        <v>F</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7" ht="13">
@@ -881,7 +881,7 @@
       </c>
       <c r="B14" s="2">
         <f>ROUND(AVERAGE(B15:B17),0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>16</v>
@@ -892,7 +892,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B15" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>17</v>
@@ -903,7 +903,7 @@
         <v>4.2</v>
       </c>
       <c r="B16" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>18</v>
@@ -926,7 +926,7 @@
       </c>
       <c r="B18" s="2">
         <f>ROUND(AVERAGE(B19:B21),0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>45</v>
@@ -937,7 +937,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B19" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>19</v>
@@ -948,7 +948,7 @@
         <v>5.2</v>
       </c>
       <c r="B20" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>20</v>
@@ -959,7 +959,7 @@
         <v>5.3</v>
       </c>
       <c r="B21" s="16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>64</v>
@@ -971,7 +971,7 @@
       </c>
       <c r="B22" s="2">
         <f>ROUND(AVERAGE(B23:B25),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>44</v>
@@ -982,7 +982,7 @@
         <v>6.1</v>
       </c>
       <c r="B23" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>21</v>
@@ -993,7 +993,7 @@
         <v>6.2</v>
       </c>
       <c r="B24" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>36</v>
@@ -1004,7 +1004,7 @@
         <v>6.3</v>
       </c>
       <c r="B25" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>55</v>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B26" s="2">
         <f>ROUND(AVERAGE(B27:B30),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>22</v>
@@ -1027,7 +1027,7 @@
         <v>7.1</v>
       </c>
       <c r="B27" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>39</v>
@@ -1038,7 +1038,7 @@
         <v>7.2</v>
       </c>
       <c r="B28" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>41</v>
@@ -1049,7 +1049,7 @@
         <v>7.3</v>
       </c>
       <c r="B29" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>40</v>
@@ -1060,7 +1060,7 @@
         <v>7.4</v>
       </c>
       <c r="B30" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>56</v>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="B31" s="2">
         <f>ROUND(AVERAGE(B32:B35),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>38</v>
@@ -1083,7 +1083,7 @@
         <v>8.1</v>
       </c>
       <c r="B32" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>42</v>
@@ -1094,7 +1094,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B33" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>57</v>
@@ -1105,7 +1105,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B34" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>43</v>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="B36" s="2">
         <f>ROUND(AVERAGE(B37:B40),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>24</v>
@@ -1172,7 +1172,7 @@
         <v>9.4</v>
       </c>
       <c r="B40" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>59</v>
@@ -1251,7 +1251,7 @@
         <v>11.2</v>
       </c>
       <c r="B47" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>62</v>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B49" s="2">
         <f>ROUND(AVERAGE(B50:B51),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>31</v>
@@ -1285,7 +1285,7 @@
         <v>12.1</v>
       </c>
       <c r="B50" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>35</v>
@@ -1296,14 +1296,14 @@
         <v>12.2</v>
       </c>
       <c r="B51" s="16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B10 B14 B18 B22 B26">
+  <conditionalFormatting sqref="B6 B1 B10 B14 B18 B22 B26">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1364,6 +1364,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2037,7 +2038,7 @@
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B10 B14 B18 B22 B26">
+  <conditionalFormatting sqref="B6 B1 B10 B14 B18 B22 B26">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>